<commit_message>
Started "Chase the Rainbow"
Added Ultrasonic distence detectors and associated code.

Started the "Chase the Rainbow"  code.

Cleaned up and removed some junk.
</commit_message>
<xml_diff>
--- a/Pin_Usage.xlsx
+++ b/Pin_Usage.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\! - Synced Docs\OneDrive\! - RaspberryPi\Git Repositorys\DalekBot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Pin</t>
   </si>
@@ -65,9 +60,6 @@
     <t>pinMotorFLForwards</t>
   </si>
   <si>
-    <t>+5</t>
-  </si>
-  <si>
     <t>+3.3</t>
   </si>
   <si>
@@ -93,13 +85,79 @@
   </si>
   <si>
     <t>Web Cam</t>
+  </si>
+  <si>
+    <t>pHat + 5</t>
+  </si>
+  <si>
+    <t>Distance +5</t>
+  </si>
+  <si>
+    <t>pHat GND</t>
+  </si>
+  <si>
+    <t>Distance GND</t>
+  </si>
+  <si>
+    <t>Pin on Dev</t>
+  </si>
+  <si>
+    <t>6 Green</t>
+  </si>
+  <si>
+    <t>3 Gray</t>
+  </si>
+  <si>
+    <t>Distance Left Echo</t>
+  </si>
+  <si>
+    <t>1 Black</t>
+  </si>
+  <si>
+    <t>Distance Left Trig</t>
+  </si>
+  <si>
+    <t>2 White</t>
+  </si>
+  <si>
+    <t>Distance Center Echo</t>
+  </si>
+  <si>
+    <t>4 Purple</t>
+  </si>
+  <si>
+    <t>Distance Center Trig</t>
+  </si>
+  <si>
+    <t>5 Blue</t>
+  </si>
+  <si>
+    <t>Distance Right Echo</t>
+  </si>
+  <si>
+    <t>Distance Right Trig</t>
+  </si>
+  <si>
+    <t>9 Red</t>
+  </si>
+  <si>
+    <t>10 Brown</t>
+  </si>
+  <si>
+    <t>Right Motor GND</t>
+  </si>
+  <si>
+    <t>Left Motor GND</t>
+  </si>
+  <si>
+    <t>Not Usable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,7 +268,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,7 +303,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -422,40 +480,47 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F1:I24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="E1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="5" customWidth="1"/>
+    <col min="1" max="4" width="5" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="5:13">
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
       <c r="G1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="5:13">
       <c r="F2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -464,12 +529,15 @@
         <v>2</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="6:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="5:13">
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="2">
         <v>3</v>
@@ -478,12 +546,12 @@
         <v>4</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="6:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="5:13">
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="2">
         <v>5</v>
@@ -492,10 +560,10 @@
         <v>6</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="6:9" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="5:13">
       <c r="G5" s="2">
         <v>7</v>
       </c>
@@ -506,9 +574,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:13">
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="2">
         <v>9</v>
@@ -520,7 +588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:13">
       <c r="F7" t="s">
         <v>1</v>
       </c>
@@ -534,7 +602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:13">
       <c r="F8" t="s">
         <v>3</v>
       </c>
@@ -545,7 +613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:13">
       <c r="F9" t="s">
         <v>2</v>
       </c>
@@ -556,9 +624,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:13">
       <c r="F10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="2">
         <v>17</v>
@@ -566,8 +634,9 @@
       <c r="H10" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="5:13">
       <c r="F11" t="s">
         <v>7</v>
       </c>
@@ -578,10 +647,10 @@
         <v>20</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="6:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="5:13">
       <c r="F12" t="s">
         <v>8</v>
       </c>
@@ -595,7 +664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:13">
       <c r="F13" t="s">
         <v>9</v>
       </c>
@@ -609,9 +678,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:13">
       <c r="F14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="2">
         <v>25</v>
@@ -623,15 +692,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:13">
+      <c r="F15" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="G15" s="2">
         <v>27</v>
       </c>
       <c r="H15" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="5:13">
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" s="2">
         <v>29</v>
       </c>
@@ -639,18 +720,39 @@
         <v>30</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="J16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10">
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G17" s="2">
         <v>31</v>
       </c>
       <c r="H17" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10">
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="G18" s="2">
         <v>33</v>
       </c>
@@ -658,10 +760,16 @@
         <v>34</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10">
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G19" s="2">
         <v>35</v>
       </c>
@@ -669,7 +777,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:10">
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G20" s="2">
         <v>37</v>
       </c>
@@ -677,9 +791,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:10">
       <c r="F21" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="G21" s="2">
         <v>39</v>
@@ -688,23 +802,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:10">
       <c r="F23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" t="s">
         <v>18</v>
       </c>
-      <c r="H23" t="s">
+    </row>
+    <row r="24" spans="5:10">
+      <c r="G24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>20</v>
-      </c>
-      <c r="H24" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>